<commit_message>
poruseni zakona o rejstricich
</commit_message>
<xml_diff>
--- a/spisy/2015/20-prehled-o-mestskych-firmach/dozorci-rady.xlsx
+++ b/spisy/2015/20-prehled-o-mestskych-firmach/dozorci-rady.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="965" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="podrobnosti" sheetId="1" state="visible" r:id="rId2"/>
@@ -555,10 +555,10 @@
     <t>ČSSD (23)</t>
   </si>
   <si>
-    <t>Trojkoalice (18)</t>
-  </si>
-  <si>
-    <t>TOP 09 (9)</t>
+    <t>Trojkoalice (19)</t>
+  </si>
+  <si>
+    <t>TOP 09 (8)</t>
   </si>
   <si>
     <t>ODS (2)</t>
@@ -592,19 +592,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <b val="true"/>
@@ -674,8 +671,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -781,7 +777,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -879,10 +875,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1022,7 +1014,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1154,79 +1146,6 @@
             </c:spPr>
           </c:dPt>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="6"/>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="7"/>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLblPos val="bestFit"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1245,10 +1164,10 @@
                   <c:v>ČSSD (23)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Trojkoalice (18)</c:v>
+                  <c:v>Trojkoalice (19)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>TOP 09 (9)</c:v>
+                  <c:v>TOP 09 (8)</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>ODS (2)</c:v>
@@ -1278,10 +1197,10 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2</c:v>
@@ -1338,15 +1257,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>14040</xdr:colOff>
+      <xdr:colOff>41040</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>105840</xdr:rowOff>
+      <xdr:rowOff>37080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>738000</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>65880</xdr:rowOff>
+      <xdr:colOff>764640</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1354,8 +1273,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4208760" y="3779640"/>
-        <a:ext cx="4758840" cy="3634200"/>
+        <a:off x="5328000" y="3586680"/>
+        <a:ext cx="5809320" cy="3809160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1375,29 +1294,29 @@
   </sheetPr>
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.9081632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="16.0918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.2704081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.2755102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.2704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.9081632653061"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.5408163265306"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.6377551020408"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.8163265306122"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.3673469387755"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.9948979591837"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.0051020408163"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.0918367346939"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.36224489795918"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.7244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.54081632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.9068825910931"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="16.0971659919028"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.2672064777328"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.2753036437247"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.2753036437247"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3522267206478"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.9109311740891"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.5465587044534"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.6396761133603"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.8178137651822"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.3684210526316"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.9959514170041"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.004048582996"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.0971659919028"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.36437246963563"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.7246963562753"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.54251012145749"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1623,7 +1542,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>43</v>
       </c>
@@ -1639,7 +1558,7 @@
       <c r="E8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="6" t="s">
         <v>46</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -2428,53 +2347,53 @@
       <c r="A34" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="B34" s="25"/>
+      <c r="B34" s="22"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="26" t="s">
+      <c r="A35" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="B35" s="25"/>
+      <c r="B35" s="22"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="B36" s="25"/>
+      <c r="B36" s="22"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="28" t="s">
+      <c r="A37" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="B37" s="25"/>
+      <c r="B37" s="22"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="B38" s="25"/>
+      <c r="B38" s="22"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="B39" s="25"/>
+      <c r="B39" s="22"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="25"/>
-      <c r="B40" s="25"/>
+      <c r="A40" s="22"/>
+      <c r="B40" s="22"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="31" t="s">
+      <c r="A41" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="B41" s="32"/>
+      <c r="B41" s="31"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="33" t="s">
+      <c r="A42" s="32" t="s">
         <v>175</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="22"/>
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
@@ -2499,43 +2418,43 @@
   </sheetPr>
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9132653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.3622448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.9132653061224"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4540816326531"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.1734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.54081632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.914979757085"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1821862348178"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.3603238866397"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1821862348178"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0971659919028"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.914979757085"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4534412955466"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.54251012145749"/>
   </cols>
   <sheetData>
-    <row r="1" s="41" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="34" t="s">
+    <row r="1" s="40" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="39" t="s">
         <v>183</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -2550,10 +2469,10 @@
         <v>23</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>2</v>
@@ -2652,7 +2571,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>42</v>
       </c>
@@ -2663,13 +2582,13 @@
         <v>98</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -2680,13 +2599,13 @@
         <v>31</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -2697,13 +2616,13 @@
         <v>47</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
@@ -2714,13 +2633,13 @@
         <v>39</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>50</v>
       </c>
@@ -2730,14 +2649,11 @@
       <c r="C11" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>114</v>
-      </c>
       <c r="H11" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
         <v>53</v>
       </c>
@@ -2751,7 +2667,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
@@ -2765,7 +2681,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
@@ -2779,7 +2695,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
@@ -2793,7 +2709,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
         <v>92</v>
       </c>
@@ -2807,7 +2723,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
         <v>94</v>
       </c>
@@ -2821,7 +2737,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
         <v>92</v>
       </c>
@@ -2835,7 +2751,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
         <v>53</v>
       </c>
@@ -2849,7 +2765,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
         <v>6</v>
       </c>
@@ -2863,15 +2779,18 @@
         <v>145</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
         <v>148</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
         <v>161</v>
       </c>
@@ -2879,7 +2798,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
         <v>45</v>
       </c>
@@ -2887,7 +2806,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
         <v>52</v>
       </c>
@@ -2895,7 +2814,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
         <v>44</v>
       </c>
@@ -2903,12 +2822,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
         <v>79</v>
       </c>
@@ -2918,92 +2837,92 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="18" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
         <v>40</v>
       </c>

</xml_diff>